<commit_message>
circuit stats & correct ang
</commit_message>
<xml_diff>
--- a/data/results_ibm-kingston.xlsx
+++ b/data/results_ibm-kingston.xlsx
@@ -71981,7 +71981,7 @@
         <v>416</v>
       </c>
       <c r="D2752" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.5015907287597656</v>
       </c>
       <c r="E2752" t="n">
         <v>0.461</v>
@@ -72007,7 +72007,7 @@
         <v>419</v>
       </c>
       <c r="D2753" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.5015945434570312</v>
       </c>
       <c r="E2753" t="n">
         <v>0.584</v>
@@ -72033,7 +72033,7 @@
         <v>420</v>
       </c>
       <c r="D2754" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.5014686584472656</v>
       </c>
       <c r="E2754" t="n">
         <v>0.307</v>
@@ -72059,7 +72059,7 @@
         <v>421</v>
       </c>
       <c r="D2755" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.5015068054199219</v>
       </c>
       <c r="E2755" t="n">
         <v>0.532</v>
@@ -72085,7 +72085,7 @@
         <v>424</v>
       </c>
       <c r="D2756" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.5015144348144531</v>
       </c>
       <c r="E2756" t="n">
         <v>0.43</v>
@@ -72111,7 +72111,7 @@
         <v>425</v>
       </c>
       <c r="D2757" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.5015029907226562</v>
       </c>
       <c r="E2757" t="n">
         <v>0.599</v>
@@ -72137,7 +72137,7 @@
         <v>426</v>
       </c>
       <c r="D2758" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.5015068054199219</v>
       </c>
       <c r="E2758" t="n">
         <v>0.434</v>
@@ -72163,7 +72163,7 @@
         <v>428</v>
       </c>
       <c r="D2759" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.5015296936035156</v>
       </c>
       <c r="E2759" t="n">
         <v>0.531</v>
@@ -72189,7 +72189,7 @@
         <v>435</v>
       </c>
       <c r="D2760" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.5015068054199219</v>
       </c>
       <c r="E2760" t="n">
         <v>0.459</v>
@@ -72215,7 +72215,7 @@
         <v>383</v>
       </c>
       <c r="D2761" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.5015335083007812</v>
       </c>
       <c r="E2761" t="n">
         <v>0.636</v>
@@ -72241,7 +72241,7 @@
         <v>404</v>
       </c>
       <c r="D2762" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.5015983581542969</v>
       </c>
       <c r="E2762" t="n">
         <v>0.678</v>
@@ -72267,7 +72267,7 @@
         <v>406</v>
       </c>
       <c r="D2763" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.5015220642089844</v>
       </c>
       <c r="E2763" t="n">
         <v>0.25</v>
@@ -72293,7 +72293,7 @@
         <v>411</v>
       </c>
       <c r="D2764" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.5015983581542969</v>
       </c>
       <c r="E2764" t="n">
         <v>0.727</v>
@@ -72319,7 +72319,7 @@
         <v>416</v>
       </c>
       <c r="D2765" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.5014839172363281</v>
       </c>
       <c r="E2765" t="n">
         <v>0.713</v>
@@ -72345,7 +72345,7 @@
         <v>419</v>
       </c>
       <c r="D2766" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.5015640258789062</v>
       </c>
       <c r="E2766" t="n">
         <v>0.646</v>
@@ -72371,7 +72371,7 @@
         <v>420</v>
       </c>
       <c r="D2767" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.5015106201171875</v>
       </c>
       <c r="E2767" t="n">
         <v>0.668</v>
@@ -72397,7 +72397,7 @@
         <v>421</v>
       </c>
       <c r="D2768" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.5015373229980469</v>
       </c>
       <c r="E2768" t="n">
         <v>0.473</v>
@@ -72423,7 +72423,7 @@
         <v>424</v>
       </c>
       <c r="D2769" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.5015983581542969</v>
       </c>
       <c r="E2769" t="n">
         <v>0.319</v>
@@ -72449,7 +72449,7 @@
         <v>425</v>
       </c>
       <c r="D2770" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.5016365051269531</v>
       </c>
       <c r="E2770" t="n">
         <v>0.63</v>
@@ -72475,7 +72475,7 @@
         <v>426</v>
       </c>
       <c r="D2771" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.5015983581542969</v>
       </c>
       <c r="E2771" t="n">
         <v>0.653</v>
@@ -72501,7 +72501,7 @@
         <v>428</v>
       </c>
       <c r="D2772" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.5015068054199219</v>
       </c>
       <c r="E2772" t="n">
         <v>0.694</v>
@@ -72527,7 +72527,7 @@
         <v>435</v>
       </c>
       <c r="D2773" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.5015029907226562</v>
       </c>
       <c r="E2773" t="n">
         <v>0.6899999999999999</v>
@@ -72553,7 +72553,7 @@
         <v>404</v>
       </c>
       <c r="D2774" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.5016021728515625</v>
       </c>
       <c r="E2774" t="n">
         <v>0.585</v>
@@ -72579,7 +72579,7 @@
         <v>406</v>
       </c>
       <c r="D2775" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.5015678405761719</v>
       </c>
       <c r="E2775" t="n">
         <v>0.176</v>
@@ -72605,7 +72605,7 @@
         <v>411</v>
       </c>
       <c r="D2776" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.5015830993652344</v>
       </c>
       <c r="E2776" t="n">
         <v>0.661</v>
@@ -72631,7 +72631,7 @@
         <v>416</v>
       </c>
       <c r="D2777" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.5016212463378906</v>
       </c>
       <c r="E2777" t="n">
         <v>0.667</v>
@@ -72657,7 +72657,7 @@
         <v>419</v>
       </c>
       <c r="D2778" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.5015716552734375</v>
       </c>
       <c r="E2778" t="n">
         <v>0.612</v>
@@ -72683,7 +72683,7 @@
         <v>420</v>
       </c>
       <c r="D2779" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.5015869140625</v>
       </c>
       <c r="E2779" t="n">
         <v>0.51</v>
@@ -72709,7 +72709,7 @@
         <v>421</v>
       </c>
       <c r="D2780" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.501617431640625</v>
       </c>
       <c r="E2780" t="n">
         <v>0.575</v>
@@ -72735,7 +72735,7 @@
         <v>424</v>
       </c>
       <c r="D2781" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.5015487670898438</v>
       </c>
       <c r="E2781" t="n">
         <v>0.395</v>
@@ -72761,7 +72761,7 @@
         <v>425</v>
       </c>
       <c r="D2782" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.5015678405761719</v>
       </c>
       <c r="E2782" t="n">
         <v>0.648</v>
@@ -72787,7 +72787,7 @@
         <v>426</v>
       </c>
       <c r="D2783" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.5016059875488281</v>
       </c>
       <c r="E2783" t="n">
         <v>0.585</v>
@@ -72813,7 +72813,7 @@
         <v>428</v>
       </c>
       <c r="D2784" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.5016212463378906</v>
       </c>
       <c r="E2784" t="n">
         <v>0.681</v>
@@ -72839,7 +72839,7 @@
         <v>435</v>
       </c>
       <c r="D2785" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.5015525817871094</v>
       </c>
       <c r="E2785" t="n">
         <v>0.66</v>
@@ -72865,7 +72865,7 @@
         <v>406</v>
       </c>
       <c r="D2786" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.50152587890625</v>
       </c>
       <c r="E2786" t="n">
         <v>0.349</v>
@@ -72891,7 +72891,7 @@
         <v>411</v>
       </c>
       <c r="D2787" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.5016136169433594</v>
       </c>
       <c r="E2787" t="n">
         <v>0.66</v>
@@ -72917,7 +72917,7 @@
         <v>416</v>
       </c>
       <c r="D2788" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.5015716552734375</v>
       </c>
       <c r="E2788" t="n">
         <v>0.6870000000000001</v>
@@ -72943,7 +72943,7 @@
         <v>419</v>
       </c>
       <c r="D2789" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.5015182495117188</v>
       </c>
       <c r="E2789" t="n">
         <v>0.626</v>
@@ -72969,7 +72969,7 @@
         <v>420</v>
       </c>
       <c r="D2790" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.5016250610351562</v>
       </c>
       <c r="E2790" t="n">
         <v>0.67</v>
@@ -72995,7 +72995,7 @@
         <v>421</v>
       </c>
       <c r="D2791" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.5015449523925781</v>
       </c>
       <c r="E2791" t="n">
         <v>0.427</v>
@@ -73021,7 +73021,7 @@
         <v>424</v>
       </c>
       <c r="D2792" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.5015869140625</v>
       </c>
       <c r="E2792" t="n">
         <v>0.41</v>
@@ -73047,7 +73047,7 @@
         <v>425</v>
       </c>
       <c r="D2793" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.5016098022460938</v>
       </c>
       <c r="E2793" t="n">
         <v>0.626</v>
@@ -73073,7 +73073,7 @@
         <v>426</v>
       </c>
       <c r="D2794" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.5015716552734375</v>
       </c>
       <c r="E2794" t="n">
         <v>0.6830000000000001</v>
@@ -73099,7 +73099,7 @@
         <v>428</v>
       </c>
       <c r="D2795" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.5016059875488281</v>
       </c>
       <c r="E2795" t="n">
         <v>0.6850000000000001</v>
@@ -73125,7 +73125,7 @@
         <v>435</v>
       </c>
       <c r="D2796" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.5015907287597656</v>
       </c>
       <c r="E2796" t="n">
         <v>0.695</v>
@@ -73151,7 +73151,7 @@
         <v>411</v>
       </c>
       <c r="D2797" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.5015068054199219</v>
       </c>
       <c r="E2797" t="n">
         <v>0.252</v>
@@ -73177,7 +73177,7 @@
         <v>416</v>
       </c>
       <c r="D2798" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.5015220642089844</v>
       </c>
       <c r="E2798" t="n">
         <v>0.267</v>
@@ -73203,7 +73203,7 @@
         <v>419</v>
       </c>
       <c r="D2799" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.5015869140625</v>
       </c>
       <c r="E2799" t="n">
         <v>0.287</v>
@@ -73229,7 +73229,7 @@
         <v>420</v>
       </c>
       <c r="D2800" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.5015068054199219</v>
       </c>
       <c r="E2800" t="n">
         <v>0.281</v>
@@ -73255,7 +73255,7 @@
         <v>421</v>
       </c>
       <c r="D2801" t="n">
-        <v>0.5019073486328125</v>
+        <v>0.5015449523925781</v>
       </c>
       <c r="E2801" t="n">
         <v>0.077</v>

</xml_diff>

<commit_message>
revert tuning curve scaling/sampling to quantum jobs
the pipeline
1. final_preprocessing
2. final_prepare_quantum_circuits
3. final_simulated_circuits
4. final_make_mitiq_circuits (in separate env)
5. jobs_ibmq
</commit_message>
<xml_diff>
--- a/data/results_ibm-kingston.xlsx
+++ b/data/results_ibm-kingston.xlsx
@@ -71981,7 +71981,7 @@
         <v>416</v>
       </c>
       <c r="D2752" t="n">
-        <v>0.5015907287597656</v>
+        <v>0.5013465881347656</v>
       </c>
       <c r="E2752" t="n">
         <v>0.461</v>
@@ -72007,7 +72007,7 @@
         <v>419</v>
       </c>
       <c r="D2753" t="n">
-        <v>0.5015945434570312</v>
+        <v>0.5013618469238281</v>
       </c>
       <c r="E2753" t="n">
         <v>0.584</v>
@@ -72033,7 +72033,7 @@
         <v>420</v>
       </c>
       <c r="D2754" t="n">
-        <v>0.5014686584472656</v>
+        <v>0.5013351440429688</v>
       </c>
       <c r="E2754" t="n">
         <v>0.307</v>
@@ -72059,7 +72059,7 @@
         <v>421</v>
       </c>
       <c r="D2755" t="n">
-        <v>0.5015068054199219</v>
+        <v>0.5012397766113281</v>
       </c>
       <c r="E2755" t="n">
         <v>0.532</v>
@@ -72085,7 +72085,7 @@
         <v>424</v>
       </c>
       <c r="D2756" t="n">
-        <v>0.5015144348144531</v>
+        <v>0.5011863708496094</v>
       </c>
       <c r="E2756" t="n">
         <v>0.43</v>
@@ -72111,7 +72111,7 @@
         <v>425</v>
       </c>
       <c r="D2757" t="n">
-        <v>0.5015029907226562</v>
+        <v>0.5013618469238281</v>
       </c>
       <c r="E2757" t="n">
         <v>0.599</v>
@@ -72137,7 +72137,7 @@
         <v>426</v>
       </c>
       <c r="D2758" t="n">
-        <v>0.5015068054199219</v>
+        <v>0.5011978149414062</v>
       </c>
       <c r="E2758" t="n">
         <v>0.434</v>
@@ -72163,7 +72163,7 @@
         <v>428</v>
       </c>
       <c r="D2759" t="n">
-        <v>0.5015296936035156</v>
+        <v>0.5012664794921875</v>
       </c>
       <c r="E2759" t="n">
         <v>0.531</v>
@@ -72189,7 +72189,7 @@
         <v>435</v>
       </c>
       <c r="D2760" t="n">
-        <v>0.5015068054199219</v>
+        <v>0.5011863708496094</v>
       </c>
       <c r="E2760" t="n">
         <v>0.459</v>
@@ -72215,7 +72215,7 @@
         <v>383</v>
       </c>
       <c r="D2761" t="n">
-        <v>0.5015335083007812</v>
+        <v>0.5015296936035156</v>
       </c>
       <c r="E2761" t="n">
         <v>0.636</v>
@@ -72241,7 +72241,7 @@
         <v>404</v>
       </c>
       <c r="D2762" t="n">
-        <v>0.5015983581542969</v>
+        <v>0.5014686584472656</v>
       </c>
       <c r="E2762" t="n">
         <v>0.678</v>
@@ -72267,7 +72267,7 @@
         <v>406</v>
       </c>
       <c r="D2763" t="n">
-        <v>0.5015220642089844</v>
+        <v>0.501007080078125</v>
       </c>
       <c r="E2763" t="n">
         <v>0.25</v>
@@ -72293,7 +72293,7 @@
         <v>411</v>
       </c>
       <c r="D2764" t="n">
-        <v>0.5015983581542969</v>
+        <v>0.5014991760253906</v>
       </c>
       <c r="E2764" t="n">
         <v>0.727</v>
@@ -72319,7 +72319,7 @@
         <v>416</v>
       </c>
       <c r="D2765" t="n">
-        <v>0.5014839172363281</v>
+        <v>0.5014915466308594</v>
       </c>
       <c r="E2765" t="n">
         <v>0.713</v>
@@ -72345,7 +72345,7 @@
         <v>419</v>
       </c>
       <c r="D2766" t="n">
-        <v>0.5015640258789062</v>
+        <v>0.5014877319335938</v>
       </c>
       <c r="E2766" t="n">
         <v>0.646</v>
@@ -72371,7 +72371,7 @@
         <v>420</v>
       </c>
       <c r="D2767" t="n">
-        <v>0.5015106201171875</v>
+        <v>0.501495361328125</v>
       </c>
       <c r="E2767" t="n">
         <v>0.668</v>
@@ -72397,7 +72397,7 @@
         <v>421</v>
       </c>
       <c r="D2768" t="n">
-        <v>0.5015373229980469</v>
+        <v>0.5014877319335938</v>
       </c>
       <c r="E2768" t="n">
         <v>0.473</v>
@@ -72423,7 +72423,7 @@
         <v>424</v>
       </c>
       <c r="D2769" t="n">
-        <v>0.5015983581542969</v>
+        <v>0.5013923645019531</v>
       </c>
       <c r="E2769" t="n">
         <v>0.319</v>
@@ -72449,7 +72449,7 @@
         <v>425</v>
       </c>
       <c r="D2770" t="n">
-        <v>0.5016365051269531</v>
+        <v>0.5016136169433594</v>
       </c>
       <c r="E2770" t="n">
         <v>0.63</v>
@@ -72475,7 +72475,7 @@
         <v>426</v>
       </c>
       <c r="D2771" t="n">
-        <v>0.5015983581542969</v>
+        <v>0.5015296936035156</v>
       </c>
       <c r="E2771" t="n">
         <v>0.653</v>
@@ -72501,7 +72501,7 @@
         <v>428</v>
       </c>
       <c r="D2772" t="n">
-        <v>0.5015068054199219</v>
+        <v>0.5015678405761719</v>
       </c>
       <c r="E2772" t="n">
         <v>0.694</v>
@@ -72527,7 +72527,7 @@
         <v>435</v>
       </c>
       <c r="D2773" t="n">
-        <v>0.5015029907226562</v>
+        <v>0.5015068054199219</v>
       </c>
       <c r="E2773" t="n">
         <v>0.6899999999999999</v>
@@ -72553,7 +72553,7 @@
         <v>404</v>
       </c>
       <c r="D2774" t="n">
-        <v>0.5016021728515625</v>
+        <v>0.5015373229980469</v>
       </c>
       <c r="E2774" t="n">
         <v>0.585</v>
@@ -72579,7 +72579,7 @@
         <v>406</v>
       </c>
       <c r="D2775" t="n">
-        <v>0.5015678405761719</v>
+        <v>0.5009994506835938</v>
       </c>
       <c r="E2775" t="n">
         <v>0.176</v>
@@ -72605,7 +72605,7 @@
         <v>411</v>
       </c>
       <c r="D2776" t="n">
-        <v>0.5015830993652344</v>
+        <v>0.5015792846679688</v>
       </c>
       <c r="E2776" t="n">
         <v>0.661</v>
@@ -72631,7 +72631,7 @@
         <v>416</v>
       </c>
       <c r="D2777" t="n">
-        <v>0.5016212463378906</v>
+        <v>0.5015716552734375</v>
       </c>
       <c r="E2777" t="n">
         <v>0.667</v>
@@ -72657,7 +72657,7 @@
         <v>419</v>
       </c>
       <c r="D2778" t="n">
-        <v>0.5015716552734375</v>
+        <v>0.5015144348144531</v>
       </c>
       <c r="E2778" t="n">
         <v>0.612</v>
@@ -72683,7 +72683,7 @@
         <v>420</v>
       </c>
       <c r="D2779" t="n">
-        <v>0.5015869140625</v>
+        <v>0.5015449523925781</v>
       </c>
       <c r="E2779" t="n">
         <v>0.51</v>
@@ -72709,7 +72709,7 @@
         <v>421</v>
       </c>
       <c r="D2780" t="n">
-        <v>0.501617431640625</v>
+        <v>0.5015220642089844</v>
       </c>
       <c r="E2780" t="n">
         <v>0.575</v>
@@ -72735,7 +72735,7 @@
         <v>424</v>
       </c>
       <c r="D2781" t="n">
-        <v>0.5015487670898438</v>
+        <v>0.5014495849609375</v>
       </c>
       <c r="E2781" t="n">
         <v>0.395</v>
@@ -72761,7 +72761,7 @@
         <v>425</v>
       </c>
       <c r="D2782" t="n">
-        <v>0.5015678405761719</v>
+        <v>0.5016136169433594</v>
       </c>
       <c r="E2782" t="n">
         <v>0.648</v>
@@ -72787,7 +72787,7 @@
         <v>426</v>
       </c>
       <c r="D2783" t="n">
-        <v>0.5016059875488281</v>
+        <v>0.5015182495117188</v>
       </c>
       <c r="E2783" t="n">
         <v>0.585</v>
@@ -72813,7 +72813,7 @@
         <v>428</v>
       </c>
       <c r="D2784" t="n">
-        <v>0.5016212463378906</v>
+        <v>0.5015640258789062</v>
       </c>
       <c r="E2784" t="n">
         <v>0.681</v>
@@ -72839,7 +72839,7 @@
         <v>435</v>
       </c>
       <c r="D2785" t="n">
-        <v>0.5015525817871094</v>
+        <v>0.5015716552734375</v>
       </c>
       <c r="E2785" t="n">
         <v>0.66</v>
@@ -72865,7 +72865,7 @@
         <v>406</v>
       </c>
       <c r="D2786" t="n">
-        <v>0.50152587890625</v>
+        <v>0.5011367797851562</v>
       </c>
       <c r="E2786" t="n">
         <v>0.349</v>
@@ -72891,7 +72891,7 @@
         <v>411</v>
       </c>
       <c r="D2787" t="n">
-        <v>0.5016136169433594</v>
+        <v>0.501556396484375</v>
       </c>
       <c r="E2787" t="n">
         <v>0.66</v>
@@ -72917,7 +72917,7 @@
         <v>416</v>
       </c>
       <c r="D2788" t="n">
-        <v>0.5015716552734375</v>
+        <v>0.5015449523925781</v>
       </c>
       <c r="E2788" t="n">
         <v>0.6870000000000001</v>
@@ -72943,7 +72943,7 @@
         <v>419</v>
       </c>
       <c r="D2789" t="n">
-        <v>0.5015182495117188</v>
+        <v>0.5016098022460938</v>
       </c>
       <c r="E2789" t="n">
         <v>0.626</v>
@@ -72969,7 +72969,7 @@
         <v>420</v>
       </c>
       <c r="D2790" t="n">
-        <v>0.5016250610351562</v>
+        <v>0.5015449523925781</v>
       </c>
       <c r="E2790" t="n">
         <v>0.67</v>
@@ -72995,7 +72995,7 @@
         <v>421</v>
       </c>
       <c r="D2791" t="n">
-        <v>0.5015449523925781</v>
+        <v>0.5014762878417969</v>
       </c>
       <c r="E2791" t="n">
         <v>0.427</v>
@@ -73021,7 +73021,7 @@
         <v>424</v>
       </c>
       <c r="D2792" t="n">
-        <v>0.5015869140625</v>
+        <v>0.5014762878417969</v>
       </c>
       <c r="E2792" t="n">
         <v>0.41</v>
@@ -73047,7 +73047,7 @@
         <v>425</v>
       </c>
       <c r="D2793" t="n">
-        <v>0.5016098022460938</v>
+        <v>0.5015640258789062</v>
       </c>
       <c r="E2793" t="n">
         <v>0.626</v>
@@ -73073,7 +73073,7 @@
         <v>426</v>
       </c>
       <c r="D2794" t="n">
-        <v>0.5015716552734375</v>
+        <v>0.5015144348144531</v>
       </c>
       <c r="E2794" t="n">
         <v>0.6830000000000001</v>
@@ -73099,7 +73099,7 @@
         <v>428</v>
       </c>
       <c r="D2795" t="n">
-        <v>0.5016059875488281</v>
+        <v>0.5015754699707031</v>
       </c>
       <c r="E2795" t="n">
         <v>0.6850000000000001</v>
@@ -73125,7 +73125,7 @@
         <v>435</v>
       </c>
       <c r="D2796" t="n">
-        <v>0.5015907287597656</v>
+        <v>0.5015487670898438</v>
       </c>
       <c r="E2796" t="n">
         <v>0.695</v>
@@ -73151,7 +73151,7 @@
         <v>411</v>
       </c>
       <c r="D2797" t="n">
-        <v>0.5015068054199219</v>
+        <v>0.5012435913085938</v>
       </c>
       <c r="E2797" t="n">
         <v>0.252</v>
@@ -73177,7 +73177,7 @@
         <v>416</v>
       </c>
       <c r="D2798" t="n">
-        <v>0.5015220642089844</v>
+        <v>0.50128173828125</v>
       </c>
       <c r="E2798" t="n">
         <v>0.267</v>
@@ -73203,7 +73203,7 @@
         <v>419</v>
       </c>
       <c r="D2799" t="n">
-        <v>0.5015869140625</v>
+        <v>0.5013465881347656</v>
       </c>
       <c r="E2799" t="n">
         <v>0.287</v>
@@ -73229,7 +73229,7 @@
         <v>420</v>
       </c>
       <c r="D2800" t="n">
-        <v>0.5015068054199219</v>
+        <v>0.5012435913085938</v>
       </c>
       <c r="E2800" t="n">
         <v>0.281</v>
@@ -73255,7 +73255,7 @@
         <v>421</v>
       </c>
       <c r="D2801" t="n">
-        <v>0.5015449523925781</v>
+        <v>0.5010261535644531</v>
       </c>
       <c r="E2801" t="n">
         <v>0.077</v>

</xml_diff>